<commit_message>
update data & plotssss
</commit_message>
<xml_diff>
--- a/01_studies/01_Laborstudie ProVisioNET/Fitbit/Heart Rate.xlsx
+++ b/01_studies/01_Laborstudie ProVisioNET/Fitbit/Heart Rate.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mk99feta\OneDrive\Dokumente\GitHub\Mandy-PhD\01_studies\01_Laborstudie ProVisioNET\Fitbit\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/505858402c07da9d/Dokumente/GitHub/Mandy-PhD/01_studies/01_Laborstudie ProVisioNET/Fitbit/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="15" documentId="14_{EB90DCE2-D67E-48F2-852C-6F2834FAA272}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{F1C6EF37-B940-4B1F-9ADF-E9E6AC6D4249}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{639708B7-9CE1-4A0A-8250-C1C28EDB4545}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="504" windowWidth="28800" windowHeight="16236" xr2:uid="{4F0FB0B0-39D8-154D-B13B-3B537C5CF837}"/>
   </bookViews>
@@ -5147,7 +5147,7 @@
         <v>754</v>
       </c>
       <c r="H22" s="6">
-        <f t="shared" ref="H22:H43" si="0">G22-F22</f>
+        <f t="shared" ref="H22:H44" si="0">G22-F22</f>
         <v>567</v>
       </c>
       <c r="I22" s="4">
@@ -5788,9 +5788,34 @@
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="F44" s="6"/>
-      <c r="G44" s="6"/>
-      <c r="H44" s="6"/>
+      <c r="A44">
+        <v>128</v>
+      </c>
+      <c r="B44" s="2">
+        <v>0.62777777777777777</v>
+      </c>
+      <c r="C44" s="7">
+        <v>0.63472222222222219</v>
+      </c>
+      <c r="D44" s="7">
+        <v>0.6479166666666667</v>
+      </c>
+      <c r="E44" s="7">
+        <v>0.69791666666666663</v>
+      </c>
+      <c r="F44" s="6">
+        <v>23</v>
+      </c>
+      <c r="G44" s="6">
+        <v>101</v>
+      </c>
+      <c r="H44" s="6">
+        <f t="shared" si="0"/>
+        <v>78</v>
+      </c>
+      <c r="I44" s="4">
+        <v>44768</v>
+      </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.3">
       <c r="F45" s="6"/>

</xml_diff>

<commit_message>
FITBIT upload case 134
</commit_message>
<xml_diff>
--- a/01_studies/01_Laborstudie ProVisioNET/Fitbit/Heart Rate.xlsx
+++ b/01_studies/01_Laborstudie ProVisioNET/Fitbit/Heart Rate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mk99feta\OneDrive\Dokumente\GitHub\Mandy-PhD\01_studies\01_Laborstudie ProVisioNET\Fitbit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="17" documentId="14_{97507877-EA25-40E1-B809-FCC1AA98D13D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{10542DDB-8A6B-485A-A73E-EB7B956D7431}"/>
+  <xr:revisionPtr revIDLastSave="19" documentId="14_{97507877-EA25-40E1-B809-FCC1AA98D13D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{5B06A5D9-129B-454D-8896-2794F66DD2F2}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="504" windowWidth="28800" windowHeight="16236" xr2:uid="{4F0FB0B0-39D8-154D-B13B-3B537C5CF837}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>ID participant</t>
   </si>
@@ -67,6 +67,9 @@
   </si>
   <si>
     <t>no steps</t>
+  </si>
+  <si>
+    <t>11:20:00</t>
   </si>
 </sst>
 </file>
@@ -163,7 +166,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -178,6 +181,10 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -404,7 +411,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp57.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp58.xml><?xml version="1.0" encoding="utf-8"?>
@@ -443,6 +450,22 @@
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
+<file path=xl/ctrlProps/ctrlProp66.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp67.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp68.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp69.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
 <file path=xl/ctrlProps/ctrlProp7.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
@@ -2814,8 +2837,8 @@
         <xdr:to>
           <xdr:col>10</xdr:col>
           <xdr:colOff>0</xdr:colOff>
-          <xdr:row>29</xdr:row>
-          <xdr:rowOff>205740</xdr:rowOff>
+          <xdr:row>30</xdr:row>
+          <xdr:rowOff>4156</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2881,8 +2904,8 @@
         <xdr:to>
           <xdr:col>10</xdr:col>
           <xdr:colOff>0</xdr:colOff>
-          <xdr:row>30</xdr:row>
-          <xdr:rowOff>205740</xdr:rowOff>
+          <xdr:row>31</xdr:row>
+          <xdr:rowOff>4157</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2948,8 +2971,8 @@
         <xdr:to>
           <xdr:col>10</xdr:col>
           <xdr:colOff>0</xdr:colOff>
-          <xdr:row>31</xdr:row>
-          <xdr:rowOff>205740</xdr:rowOff>
+          <xdr:row>32</xdr:row>
+          <xdr:rowOff>4156</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -3015,8 +3038,8 @@
         <xdr:to>
           <xdr:col>10</xdr:col>
           <xdr:colOff>0</xdr:colOff>
-          <xdr:row>33</xdr:row>
-          <xdr:rowOff>205740</xdr:rowOff>
+          <xdr:row>34</xdr:row>
+          <xdr:rowOff>4157</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -3082,8 +3105,8 @@
         <xdr:to>
           <xdr:col>10</xdr:col>
           <xdr:colOff>0</xdr:colOff>
-          <xdr:row>34</xdr:row>
-          <xdr:rowOff>205740</xdr:rowOff>
+          <xdr:row>35</xdr:row>
+          <xdr:rowOff>4156</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -3149,8 +3172,8 @@
         <xdr:to>
           <xdr:col>10</xdr:col>
           <xdr:colOff>0</xdr:colOff>
-          <xdr:row>35</xdr:row>
-          <xdr:rowOff>205740</xdr:rowOff>
+          <xdr:row>36</xdr:row>
+          <xdr:rowOff>4156</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -3216,8 +3239,8 @@
         <xdr:to>
           <xdr:col>10</xdr:col>
           <xdr:colOff>0</xdr:colOff>
-          <xdr:row>36</xdr:row>
-          <xdr:rowOff>205740</xdr:rowOff>
+          <xdr:row>37</xdr:row>
+          <xdr:rowOff>4157</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -3283,8 +3306,8 @@
         <xdr:to>
           <xdr:col>10</xdr:col>
           <xdr:colOff>0</xdr:colOff>
-          <xdr:row>37</xdr:row>
-          <xdr:rowOff>205740</xdr:rowOff>
+          <xdr:row>38</xdr:row>
+          <xdr:rowOff>4156</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -3350,8 +3373,8 @@
         <xdr:to>
           <xdr:col>10</xdr:col>
           <xdr:colOff>0</xdr:colOff>
-          <xdr:row>38</xdr:row>
-          <xdr:rowOff>205740</xdr:rowOff>
+          <xdr:row>39</xdr:row>
+          <xdr:rowOff>4156</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -3417,8 +3440,8 @@
         <xdr:to>
           <xdr:col>10</xdr:col>
           <xdr:colOff>0</xdr:colOff>
-          <xdr:row>39</xdr:row>
-          <xdr:rowOff>205740</xdr:rowOff>
+          <xdr:row>40</xdr:row>
+          <xdr:rowOff>4157</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -3484,8 +3507,8 @@
         <xdr:to>
           <xdr:col>10</xdr:col>
           <xdr:colOff>0</xdr:colOff>
-          <xdr:row>41</xdr:row>
-          <xdr:rowOff>205740</xdr:rowOff>
+          <xdr:row>42</xdr:row>
+          <xdr:rowOff>4157</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -3551,8 +3574,8 @@
         <xdr:to>
           <xdr:col>10</xdr:col>
           <xdr:colOff>0</xdr:colOff>
-          <xdr:row>43</xdr:row>
-          <xdr:rowOff>205740</xdr:rowOff>
+          <xdr:row>44</xdr:row>
+          <xdr:rowOff>4156</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -3618,8 +3641,8 @@
         <xdr:to>
           <xdr:col>10</xdr:col>
           <xdr:colOff>0</xdr:colOff>
-          <xdr:row>44</xdr:row>
-          <xdr:rowOff>205740</xdr:rowOff>
+          <xdr:row>45</xdr:row>
+          <xdr:rowOff>4157</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -3685,8 +3708,8 @@
         <xdr:to>
           <xdr:col>10</xdr:col>
           <xdr:colOff>0</xdr:colOff>
-          <xdr:row>45</xdr:row>
-          <xdr:rowOff>205740</xdr:rowOff>
+          <xdr:row>46</xdr:row>
+          <xdr:rowOff>4156</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -3752,8 +3775,8 @@
         <xdr:to>
           <xdr:col>10</xdr:col>
           <xdr:colOff>0</xdr:colOff>
-          <xdr:row>46</xdr:row>
-          <xdr:rowOff>205740</xdr:rowOff>
+          <xdr:row>47</xdr:row>
+          <xdr:rowOff>4156</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -3819,8 +3842,8 @@
         <xdr:to>
           <xdr:col>10</xdr:col>
           <xdr:colOff>0</xdr:colOff>
-          <xdr:row>47</xdr:row>
-          <xdr:rowOff>205740</xdr:rowOff>
+          <xdr:row>48</xdr:row>
+          <xdr:rowOff>4157</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -3886,8 +3909,8 @@
         <xdr:to>
           <xdr:col>10</xdr:col>
           <xdr:colOff>0</xdr:colOff>
-          <xdr:row>48</xdr:row>
-          <xdr:rowOff>205740</xdr:rowOff>
+          <xdr:row>49</xdr:row>
+          <xdr:rowOff>4156</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -3953,8 +3976,8 @@
         <xdr:to>
           <xdr:col>10</xdr:col>
           <xdr:colOff>0</xdr:colOff>
-          <xdr:row>49</xdr:row>
-          <xdr:rowOff>205740</xdr:rowOff>
+          <xdr:row>50</xdr:row>
+          <xdr:rowOff>4156</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -4020,8 +4043,8 @@
         <xdr:to>
           <xdr:col>10</xdr:col>
           <xdr:colOff>0</xdr:colOff>
-          <xdr:row>50</xdr:row>
-          <xdr:rowOff>205740</xdr:rowOff>
+          <xdr:row>51</xdr:row>
+          <xdr:rowOff>4157</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -4087,8 +4110,8 @@
         <xdr:to>
           <xdr:col>10</xdr:col>
           <xdr:colOff>0</xdr:colOff>
-          <xdr:row>51</xdr:row>
-          <xdr:rowOff>205740</xdr:rowOff>
+          <xdr:row>52</xdr:row>
+          <xdr:rowOff>4156</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -4154,8 +4177,8 @@
         <xdr:to>
           <xdr:col>10</xdr:col>
           <xdr:colOff>0</xdr:colOff>
-          <xdr:row>52</xdr:row>
-          <xdr:rowOff>205740</xdr:rowOff>
+          <xdr:row>53</xdr:row>
+          <xdr:rowOff>4157</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -4221,8 +4244,8 @@
         <xdr:to>
           <xdr:col>10</xdr:col>
           <xdr:colOff>0</xdr:colOff>
-          <xdr:row>53</xdr:row>
-          <xdr:rowOff>205740</xdr:rowOff>
+          <xdr:row>54</xdr:row>
+          <xdr:rowOff>4156</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -4809,6 +4832,254 @@
         </xdr:sp>
         <xdr:clientData/>
       </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>9</xdr:col>
+          <xdr:colOff>15240</xdr:colOff>
+          <xdr:row>53</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="1217815" cy="198120"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1093" name="Check Box 69" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1093"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D0E4BA96-874A-4EA6-BD46-E4EF5229E9F8}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>9</xdr:col>
+          <xdr:colOff>15240</xdr:colOff>
+          <xdr:row>54</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="1217815" cy="198120"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1094" name="Check Box 70" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1094"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6B924131-C440-4F14-B962-E3DD4B619BC9}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>9</xdr:col>
+          <xdr:colOff>15240</xdr:colOff>
+          <xdr:row>54</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="1217815" cy="198120"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1095" name="Check Box 71" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1095"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3A8C4722-0BC6-4BDF-8A16-A822A2E6489D}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>9</xdr:col>
+          <xdr:colOff>15240</xdr:colOff>
+          <xdr:row>55</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="1217815" cy="198120"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1096" name="Check Box 72" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1096"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B70242BD-E5DE-4A18-8169-9DE8C510B69F}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
@@ -5115,8 +5386,8 @@
   <dimension ref="A1:K143"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A54" sqref="A46:XFD54"/>
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I62" sqref="I62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -6737,7 +7008,7 @@
         <v>0.69027777777777777</v>
       </c>
       <c r="E54" s="9">
-        <v>0.73749999999999993</v>
+        <v>0.72986111111111107</v>
       </c>
       <c r="F54" s="10">
         <v>43</v>
@@ -6752,19 +7023,44 @@
       <c r="I54" s="13">
         <v>44823</v>
       </c>
-      <c r="K54" s="3" t="s">
-        <v>11</v>
-      </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A55" s="6">
+        <v>220</v>
+      </c>
+      <c r="B55" s="9">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="C55" s="9">
+        <v>0.4236111111111111</v>
+      </c>
+      <c r="D55" s="14"/>
+      <c r="E55" s="15" t="s">
+        <v>14</v>
+      </c>
       <c r="F55" s="10"/>
       <c r="G55" s="10"/>
       <c r="H55" s="10"/>
+      <c r="I55" s="13">
+        <v>44833</v>
+      </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A56" s="6">
+        <v>221</v>
+      </c>
+      <c r="B56" s="9">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="E56" s="9">
+        <v>0.54166666666666663</v>
+      </c>
       <c r="F56" s="10"/>
       <c r="G56" s="10"/>
       <c r="H56" s="10"/>
+      <c r="I56" s="13">
+        <v>44833</v>
+      </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.3">
       <c r="F57" s="10"/>
@@ -8639,6 +8935,94 @@
             </control>
           </mc:Choice>
         </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1093" r:id="rId69" name="Check Box 69">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>9</xdr:col>
+                    <xdr:colOff>15240</xdr:colOff>
+                    <xdr:row>53</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>10</xdr:col>
+                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:row>54</xdr:row>
+                    <xdr:rowOff>7620</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1094" r:id="rId70" name="Check Box 70">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>9</xdr:col>
+                    <xdr:colOff>15240</xdr:colOff>
+                    <xdr:row>54</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>10</xdr:col>
+                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:row>55</xdr:row>
+                    <xdr:rowOff>7620</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1095" r:id="rId71" name="Check Box 71">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>9</xdr:col>
+                    <xdr:colOff>15240</xdr:colOff>
+                    <xdr:row>54</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>10</xdr:col>
+                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:row>55</xdr:row>
+                    <xdr:rowOff>7620</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1096" r:id="rId72" name="Check Box 72">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>9</xdr:col>
+                    <xdr:colOff>15240</xdr:colOff>
+                    <xdr:row>55</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>10</xdr:col>
+                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:row>56</xdr:row>
+                    <xdr:rowOff>7620</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
       </controls>
     </mc:Choice>
   </mc:AlternateContent>

</xml_diff>